<commit_message>
some minor changes to Itsari
</commit_message>
<xml_diff>
--- a/lists/itsari.xlsx
+++ b/lists/itsari.xlsx
@@ -11,12 +11,12 @@
     <sheet name="lexcauc" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$A$1:$AC$2075</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$A$1:$J$2075</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Excel_BuiltIn__FilterDatabase" vbProcedure="false">lexcauc!$H$1:$J$2660</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters_1" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="parameters_2" vbProcedure="false">#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$A$1:$J$2075</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">lexcauc!$A$1:$AC$2075</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25026,9 +25026,7 @@
     <cellStyle name="Warning 3" xfId="85"/>
   </cellStyles>
   <dxfs count="1">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-    </dxf>
+    <dxf/>
   </dxfs>
   <colors>
     <indexedColors>
@@ -25105,12 +25103,12 @@
   <dimension ref="A1:AMJ2078"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="K2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="K29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D44" activeCellId="0" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.15"/>
@@ -25125,9 +25123,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="14" style="3" width="11.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="28" style="0" width="11.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="14" style="3" width="11.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26536,11 +26533,11 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>37</v>
@@ -85624,7 +85621,7 @@
       <c r="J2078" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC2075"/>
+  <autoFilter ref="A1:J2075"/>
   <conditionalFormatting sqref="C1:IN1">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>LEN(TRIM(C1))&gt;0</formula>

</xml_diff>